<commit_message>
fix: duplicate value in outcome weekly values
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/outcome/1_0/1_0_weekly_rep.xlsx
+++ b/R/data/dictionaries/outcome/1_0/1_0_weekly_rep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/outcome/1_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D298BEF3-BB74-4045-9AB3-103576E2123D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2690622-FA56-1E4F-809C-559D658D5F3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t>name</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>mmhg</t>
-  </si>
-  <si>
-    <t>mU/L</t>
   </si>
   <si>
     <t>isMissing</t>
@@ -743,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG142"/>
+  <dimension ref="A1:BG141"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -769,7 +766,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
@@ -829,16 +826,16 @@
     </row>
     <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>26</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>27</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
@@ -898,14 +895,14 @@
     </row>
     <row r="3" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
@@ -965,16 +962,16 @@
     </row>
     <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>31</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
@@ -1034,16 +1031,16 @@
     </row>
     <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>33</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -1103,7 +1100,7 @@
     </row>
     <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>4</v>
@@ -1112,7 +1109,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
@@ -1172,7 +1169,7 @@
     </row>
     <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>4</v>
@@ -1181,7 +1178,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -1241,7 +1238,7 @@
     </row>
     <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>4</v>
@@ -1250,13 +1247,13 @@
         <v>5</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>4</v>
@@ -1265,13 +1262,13 @@
         <v>5</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>4</v>
@@ -1280,13 +1277,13 @@
         <v>5</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>4</v>
@@ -1295,13 +1292,13 @@
         <v>5</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="15"/>
     </row>
     <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>4</v>
@@ -1310,7 +1307,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="15"/>
     </row>
@@ -1322,7 +1319,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>41</v>
@@ -1370,22 +1367,22 @@
         <v>5</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="E16" s="15"/>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="E17" s="15"/>
     </row>
@@ -1405,88 +1402,80 @@
       <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>46</v>
-      </c>
+      <c r="A19" s="17"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
       <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="15"/>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="19"/>
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="19"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
       <c r="E23" s="15"/>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="15"/>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="19"/>
       <c r="E25" s="15"/>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="19"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
       <c r="E26" s="15"/>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="15"/>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="19"/>
       <c r="E28" s="15"/>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="19"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="15"/>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1498,16 +1487,16 @@
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
       <c r="E31" s="15"/>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="15"/>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1519,16 +1508,16 @@
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
       <c r="E34" s="15"/>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
       <c r="E35" s="15"/>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1540,16 +1529,16 @@
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
       <c r="E37" s="15"/>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
       <c r="E38" s="15"/>
     </row>
     <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1561,16 +1550,16 @@
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
       <c r="E40" s="15"/>
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
       <c r="E41" s="15"/>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1582,16 +1571,16 @@
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
       <c r="E43" s="15"/>
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
       <c r="E44" s="15"/>
     </row>
     <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1603,16 +1592,16 @@
     </row>
     <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
       <c r="E46" s="15"/>
     </row>
     <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
       <c r="E47" s="15"/>
     </row>
     <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1624,15 +1613,15 @@
     </row>
     <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="18"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
       <c r="D49" s="18"/>
       <c r="E49" s="15"/>
     </row>
     <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
       <c r="D50" s="18"/>
       <c r="E50" s="15"/>
     </row>
@@ -1645,15 +1634,15 @@
     </row>
     <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="18"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
       <c r="D52" s="18"/>
       <c r="E52" s="15"/>
     </row>
     <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="18"/>
       <c r="D53" s="18"/>
       <c r="E53" s="15"/>
     </row>
@@ -1665,227 +1654,227 @@
       <c r="E54" s="15"/>
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="17"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="18"/>
+      <c r="A55" s="18"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
       <c r="D55" s="18"/>
       <c r="E55" s="15"/>
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="18"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="18"/>
+      <c r="A56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
       <c r="E56" s="15"/>
     </row>
     <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
       <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
       <c r="E57" s="15"/>
     </row>
     <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="17"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="18"/>
+      <c r="A58" s="18"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
       <c r="D58" s="18"/>
       <c r="E58" s="15"/>
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="18"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="18"/>
+      <c r="A59" s="17"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
       <c r="E59" s="15"/>
     </row>
     <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="17"/>
       <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
       <c r="E60" s="15"/>
     </row>
     <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="17"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="18"/>
+      <c r="A61" s="18"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
       <c r="D61" s="18"/>
       <c r="E61" s="15"/>
     </row>
     <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="18"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="18"/>
+      <c r="A62" s="17"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
       <c r="E62" s="15"/>
     </row>
     <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17"/>
       <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
       <c r="E63" s="15"/>
     </row>
     <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="17"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="18"/>
+      <c r="A64" s="18"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
       <c r="D64" s="18"/>
       <c r="E64" s="15"/>
     </row>
     <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="18"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="18"/>
+      <c r="A65" s="17"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="17"/>
       <c r="E65" s="15"/>
     </row>
     <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
       <c r="E66" s="15"/>
     </row>
     <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="17"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="18"/>
+      <c r="A67" s="18"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
       <c r="D67" s="18"/>
       <c r="E67" s="15"/>
     </row>
     <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="18"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="18"/>
+      <c r="A68" s="17"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="20"/>
       <c r="E68" s="15"/>
     </row>
     <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="18"/>
-      <c r="D69" s="20"/>
+      <c r="D69" s="18"/>
       <c r="E69" s="15"/>
     </row>
     <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="17"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="18"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
       <c r="D70" s="18"/>
       <c r="E70" s="15"/>
     </row>
     <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="17"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="18"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="20"/>
       <c r="E71" s="15"/>
     </row>
     <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="17"/>
       <c r="B72" s="17"/>
       <c r="C72" s="18"/>
-      <c r="D72" s="20"/>
+      <c r="D72" s="18"/>
       <c r="E72" s="15"/>
     </row>
     <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="17"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="18"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="14"/>
       <c r="D73" s="18"/>
       <c r="E73" s="15"/>
     </row>
     <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="17"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="18"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="20"/>
       <c r="E74" s="15"/>
     </row>
     <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="17"/>
       <c r="B75" s="17"/>
       <c r="C75" s="18"/>
-      <c r="D75" s="20"/>
+      <c r="D75" s="18"/>
       <c r="E75" s="15"/>
     </row>
     <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="17"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="18"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
       <c r="D76" s="18"/>
       <c r="E76" s="15"/>
     </row>
     <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="17"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="18"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="20"/>
       <c r="E77" s="15"/>
     </row>
     <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="17"/>
       <c r="B78" s="17"/>
       <c r="C78" s="18"/>
-      <c r="D78" s="20"/>
+      <c r="D78" s="18"/>
       <c r="E78" s="15"/>
     </row>
     <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="17"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="18"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
       <c r="D79" s="18"/>
       <c r="E79" s="15"/>
     </row>
     <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="17"/>
-      <c r="B80" s="14"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="18"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="20"/>
       <c r="E80" s="15"/>
     </row>
     <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="17"/>
       <c r="B81" s="17"/>
       <c r="C81" s="18"/>
-      <c r="D81" s="20"/>
+      <c r="D81" s="18"/>
       <c r="E81" s="15"/>
     </row>
     <row r="82" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="17"/>
-      <c r="B82" s="17"/>
-      <c r="C82" s="18"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
       <c r="D82" s="18"/>
       <c r="E82" s="15"/>
     </row>
     <row r="83" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="17"/>
-      <c r="B83" s="14"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="18"/>
+      <c r="B83" s="17"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="17"/>
       <c r="E83" s="15"/>
     </row>
     <row r="84" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="17"/>
+      <c r="A84" s="18"/>
       <c r="B84" s="17"/>
       <c r="C84" s="18"/>
-      <c r="D84" s="17"/>
+      <c r="D84" s="18"/>
       <c r="E84" s="15"/>
     </row>
     <row r="85" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="18"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="18"/>
+      <c r="A85" s="17"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="14"/>
       <c r="D85" s="18"/>
       <c r="E85" s="15"/>
     </row>
     <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="17"/>
-      <c r="B86" s="14"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="18"/>
+      <c r="B86" s="17"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="20"/>
       <c r="E86" s="15"/>
     </row>
     <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1910,37 +1899,37 @@
       <c r="E89" s="15"/>
     </row>
     <row r="90" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="17"/>
+      <c r="A90" s="20"/>
       <c r="B90" s="17"/>
       <c r="C90" s="18"/>
-      <c r="D90" s="20"/>
+      <c r="D90" s="18"/>
       <c r="E90" s="15"/>
     </row>
     <row r="91" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="20"/>
       <c r="B91" s="17"/>
       <c r="C91" s="18"/>
-      <c r="D91" s="18"/>
+      <c r="D91" s="17"/>
       <c r="E91" s="15"/>
     </row>
     <row r="92" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="20"/>
       <c r="B92" s="17"/>
       <c r="C92" s="18"/>
-      <c r="D92" s="17"/>
+      <c r="D92" s="18"/>
       <c r="E92" s="15"/>
     </row>
     <row r="93" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="20"/>
-      <c r="B93" s="17"/>
-      <c r="C93" s="18"/>
+      <c r="A93" s="17"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="14"/>
       <c r="D93" s="18"/>
       <c r="E93" s="15"/>
     </row>
     <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="17"/>
-      <c r="B94" s="14"/>
-      <c r="C94" s="14"/>
+      <c r="A94" s="20"/>
+      <c r="B94" s="17"/>
+      <c r="C94" s="18"/>
       <c r="D94" s="18"/>
       <c r="E94" s="15"/>
     </row>
@@ -1959,16 +1948,16 @@
       <c r="E96" s="15"/>
     </row>
     <row r="97" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="20"/>
-      <c r="B97" s="17"/>
-      <c r="C97" s="18"/>
+      <c r="A97" s="17"/>
+      <c r="B97" s="14"/>
+      <c r="C97" s="14"/>
       <c r="D97" s="18"/>
       <c r="E97" s="15"/>
     </row>
     <row r="98" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="17"/>
-      <c r="B98" s="14"/>
-      <c r="C98" s="14"/>
+      <c r="A98" s="20"/>
+      <c r="B98" s="17"/>
+      <c r="C98" s="18"/>
       <c r="D98" s="18"/>
       <c r="E98" s="15"/>
     </row>
@@ -1983,14 +1972,14 @@
       <c r="A100" s="20"/>
       <c r="B100" s="17"/>
       <c r="C100" s="18"/>
-      <c r="D100" s="18"/>
+      <c r="D100" s="21"/>
       <c r="E100" s="15"/>
     </row>
     <row r="101" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="20"/>
       <c r="B101" s="17"/>
       <c r="C101" s="18"/>
-      <c r="D101" s="21"/>
+      <c r="D101" s="18"/>
       <c r="E101" s="15"/>
     </row>
     <row r="102" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2008,16 +1997,16 @@
       <c r="E103" s="15"/>
     </row>
     <row r="104" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="20"/>
-      <c r="B104" s="17"/>
-      <c r="C104" s="18"/>
-      <c r="D104" s="18"/>
+      <c r="A104" s="17"/>
+      <c r="B104" s="14"/>
+      <c r="C104" s="14"/>
+      <c r="D104" s="17"/>
       <c r="E104" s="15"/>
     </row>
     <row r="105" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="17"/>
-      <c r="B105" s="14"/>
-      <c r="C105" s="14"/>
+      <c r="A105" s="20"/>
+      <c r="B105" s="18"/>
+      <c r="C105" s="18"/>
       <c r="D105" s="17"/>
       <c r="E105" s="15"/>
     </row>
@@ -2074,7 +2063,7 @@
       <c r="A113" s="20"/>
       <c r="B113" s="18"/>
       <c r="C113" s="18"/>
-      <c r="D113" s="17"/>
+      <c r="D113" s="18"/>
       <c r="E113" s="15"/>
     </row>
     <row r="114" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2088,7 +2077,7 @@
       <c r="A115" s="20"/>
       <c r="B115" s="18"/>
       <c r="C115" s="18"/>
-      <c r="D115" s="18"/>
+      <c r="D115" s="17"/>
       <c r="E115" s="15"/>
     </row>
     <row r="116" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2120,9 +2109,9 @@
       <c r="E119" s="15"/>
     </row>
     <row r="120" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="20"/>
-      <c r="B120" s="18"/>
-      <c r="C120" s="18"/>
+      <c r="A120" s="17"/>
+      <c r="B120" s="17"/>
+      <c r="C120" s="17"/>
       <c r="D120" s="17"/>
       <c r="E120" s="15"/>
     </row>
@@ -2169,29 +2158,29 @@
       <c r="E126" s="15"/>
     </row>
     <row r="127" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="17"/>
       <c r="B127" s="17"/>
-      <c r="C127" s="17"/>
-      <c r="D127" s="17"/>
+      <c r="C127" s="22"/>
       <c r="E127" s="15"/>
     </row>
     <row r="128" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="17"/>
       <c r="B128" s="17"/>
-      <c r="C128" s="22"/>
+      <c r="C128" s="18"/>
+      <c r="D128" s="17"/>
       <c r="E128" s="15"/>
     </row>
     <row r="129" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="17"/>
-      <c r="B129" s="17"/>
+      <c r="A129" s="18"/>
+      <c r="B129" s="18"/>
       <c r="C129" s="18"/>
-      <c r="D129" s="17"/>
+      <c r="D129" s="18"/>
       <c r="E129" s="15"/>
     </row>
     <row r="130" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="18"/>
+      <c r="A130" s="17"/>
       <c r="B130" s="18"/>
       <c r="C130" s="18"/>
-      <c r="D130" s="18"/>
+      <c r="D130" s="17"/>
       <c r="E130" s="15"/>
     </row>
     <row r="131" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2227,7 +2216,6 @@
       <c r="B135" s="18"/>
       <c r="C135" s="18"/>
       <c r="D135" s="17"/>
-      <c r="E135" s="15"/>
     </row>
     <row r="136" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="17"/>
@@ -2237,8 +2225,8 @@
     </row>
     <row r="137" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="17"/>
-      <c r="B137" s="18"/>
-      <c r="C137" s="18"/>
+      <c r="B137" s="17"/>
+      <c r="C137" s="17"/>
       <c r="D137" s="17"/>
     </row>
     <row r="138" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2261,15 +2249,9 @@
     </row>
     <row r="141" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="17"/>
-      <c r="B141" s="17"/>
+      <c r="B141" s="18"/>
       <c r="C141" s="17"/>
-      <c r="D141" s="17"/>
-    </row>
-    <row r="142" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="17"/>
-      <c r="B142" s="18"/>
-      <c r="C142" s="17"/>
-      <c r="D142" s="20"/>
+      <c r="D141" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
@@ -2305,10 +2287,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>